<commit_message>
Adding Office365 CC (v1707) command identifiers
</commit_message>
<xml_diff>
--- a/Office 2016/Office365-Current-Channel/onenotecontrols.xlsx
+++ b/Office 2016/Office365-Current-Channel/onenotecontrols.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RibbonX-output\CC-8229-1016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RibbonX\CC-8326\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>

</xml_diff>